<commit_message>
updated with new spawner data
</commit_message>
<xml_diff>
--- a/Surveyability_Web/Daily_Precip_Discharge_Monitoring.xlsx
+++ b/Surveyability_Web/Daily_Precip_Discharge_Monitoring.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="223">
   <si>
     <t>down</t>
   </si>
@@ -1816,11 +1816,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G364"/>
+  <dimension ref="A1:G618"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A335" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E362" sqref="E362"/>
+      <pane ySplit="1" topLeftCell="A355" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E368" sqref="E368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7478,10 +7478,1340 @@
       <c r="A363" s="7">
         <v>42705</v>
       </c>
+      <c r="B363">
+        <v>0.04</v>
+      </c>
+      <c r="C363">
+        <v>0.01</v>
+      </c>
+      <c r="D363">
+        <v>0.01</v>
+      </c>
+      <c r="E363">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" s="7">
         <v>42706</v>
+      </c>
+      <c r="B364">
+        <v>0</v>
+      </c>
+      <c r="C364">
+        <v>0</v>
+      </c>
+      <c r="D364">
+        <v>0</v>
+      </c>
+      <c r="E364">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A365" s="7">
+        <v>42707</v>
+      </c>
+      <c r="B365" t="s">
+        <v>221</v>
+      </c>
+      <c r="C365" t="s">
+        <v>221</v>
+      </c>
+      <c r="D365" t="s">
+        <v>221</v>
+      </c>
+      <c r="E365" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A366" s="7">
+        <v>42708</v>
+      </c>
+      <c r="B366">
+        <v>0</v>
+      </c>
+      <c r="C366">
+        <v>0</v>
+      </c>
+      <c r="D366">
+        <v>0</v>
+      </c>
+      <c r="E366">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A367" s="7">
+        <v>42709</v>
+      </c>
+      <c r="B367">
+        <v>0</v>
+      </c>
+      <c r="C367">
+        <v>0</v>
+      </c>
+      <c r="D367">
+        <v>0</v>
+      </c>
+      <c r="E367">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A368" s="7">
+        <v>42710</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" s="7">
+        <v>42711</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" s="7">
+        <v>42712</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" s="7">
+        <v>42713</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" s="7">
+        <v>42714</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" s="7">
+        <v>42715</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" s="7">
+        <v>42716</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" s="7">
+        <v>42717</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" s="7">
+        <v>42718</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" s="7">
+        <v>42719</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" s="7">
+        <v>42720</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" s="7">
+        <v>42721</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" s="7">
+        <v>42722</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" s="7">
+        <v>42723</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" s="7">
+        <v>42724</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" s="7">
+        <v>42725</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" s="7">
+        <v>42726</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" s="7">
+        <v>42727</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" s="7">
+        <v>42728</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" s="7">
+        <v>42729</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" s="7">
+        <v>42730</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" s="7">
+        <v>42731</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" s="7">
+        <v>42732</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" s="7">
+        <v>42733</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" s="7">
+        <v>42734</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" s="7">
+        <v>42735</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" s="7">
+        <v>42736</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" s="7">
+        <v>42737</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396" s="7">
+        <v>42738</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" s="7">
+        <v>42739</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" s="7">
+        <v>42740</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399" s="7">
+        <v>42741</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" s="7">
+        <v>42742</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" s="7">
+        <v>42743</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" s="7">
+        <v>42744</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" s="7">
+        <v>42745</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" s="7">
+        <v>42746</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" s="7">
+        <v>42747</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" s="7">
+        <v>42748</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" s="7">
+        <v>42749</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" s="7">
+        <v>42750</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" s="7">
+        <v>42751</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" s="7">
+        <v>42752</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" s="7">
+        <v>42753</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" s="7">
+        <v>42754</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" s="7">
+        <v>42755</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" s="7">
+        <v>42756</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" s="7">
+        <v>42757</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" s="7">
+        <v>42758</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" s="7">
+        <v>42759</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" s="7">
+        <v>42760</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" s="7">
+        <v>42761</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" s="7">
+        <v>42762</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" s="7">
+        <v>42763</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" s="7">
+        <v>42764</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" s="7">
+        <v>42765</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" s="7">
+        <v>42766</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" s="7">
+        <v>42767</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" s="7">
+        <v>42768</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" s="7">
+        <v>42769</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" s="7">
+        <v>42770</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" s="7">
+        <v>42771</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" s="7">
+        <v>42772</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" s="7">
+        <v>42773</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" s="7">
+        <v>42774</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" s="7">
+        <v>42775</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434" s="7">
+        <v>42776</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435" s="7">
+        <v>42777</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" s="7">
+        <v>42778</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437" s="7">
+        <v>42779</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438" s="7">
+        <v>42780</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" s="7">
+        <v>42781</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" s="7">
+        <v>42782</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" s="7">
+        <v>42783</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" s="7">
+        <v>42784</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" s="7">
+        <v>42785</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" s="7">
+        <v>42786</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" s="7">
+        <v>42787</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" s="7">
+        <v>42788</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" s="7">
+        <v>42789</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" s="7">
+        <v>42790</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" s="7">
+        <v>42791</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" s="7">
+        <v>42792</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" s="7">
+        <v>42793</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" s="7">
+        <v>42794</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453" s="7">
+        <v>42795</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" s="7">
+        <v>42796</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" s="7">
+        <v>42797</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" s="7">
+        <v>42798</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457" s="7">
+        <v>42799</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A458" s="7">
+        <v>42800</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A459" s="7">
+        <v>42801</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460" s="7">
+        <v>42802</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461" s="7">
+        <v>42803</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462" s="7">
+        <v>42804</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463" s="7">
+        <v>42805</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" s="7">
+        <v>42806</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" s="7">
+        <v>42807</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" s="7">
+        <v>42808</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" s="7">
+        <v>42809</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" s="7">
+        <v>42810</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" s="7">
+        <v>42811</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" s="7">
+        <v>42812</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" s="7">
+        <v>42813</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" s="7">
+        <v>42814</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" s="7">
+        <v>42815</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" s="7">
+        <v>42816</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" s="7">
+        <v>42817</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" s="7">
+        <v>42818</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" s="7">
+        <v>42819</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" s="7">
+        <v>42820</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" s="7">
+        <v>42821</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" s="7">
+        <v>42822</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" s="7">
+        <v>42823</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" s="7">
+        <v>42824</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A483" s="7">
+        <v>42825</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A484" s="7">
+        <v>42826</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A485" s="7">
+        <v>42827</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A486" s="7">
+        <v>42828</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A487" s="7">
+        <v>42829</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A488" s="7">
+        <v>42830</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A489" s="7">
+        <v>42831</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A490" s="7">
+        <v>42832</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A491" s="7">
+        <v>42833</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A492" s="7">
+        <v>42834</v>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A493" s="7">
+        <v>42835</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A494" s="7">
+        <v>42836</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A495" s="7">
+        <v>42837</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A496" s="7">
+        <v>42838</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A497" s="7">
+        <v>42839</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A498" s="7">
+        <v>42840</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A499" s="7">
+        <v>42841</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500" s="7">
+        <v>42842</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501" s="7">
+        <v>42843</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A502" s="7">
+        <v>42844</v>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A503" s="7">
+        <v>42845</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A504" s="7">
+        <v>42846</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A505" s="7">
+        <v>42847</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A506" s="7">
+        <v>42848</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A507" s="7">
+        <v>42849</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A508" s="7">
+        <v>42850</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A509" s="7">
+        <v>42851</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A510" s="7">
+        <v>42852</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511" s="7">
+        <v>42853</v>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A512" s="7">
+        <v>42854</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A513" s="7">
+        <v>42855</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514" s="7">
+        <v>42856</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515" s="7">
+        <v>42857</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A516" s="7">
+        <v>42858</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A517" s="7">
+        <v>42859</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A518" s="7">
+        <v>42860</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A519" s="7">
+        <v>42861</v>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A520" s="7">
+        <v>42862</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A521" s="7">
+        <v>42863</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522" s="7">
+        <v>42864</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523" s="7">
+        <v>42865</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524" s="7">
+        <v>42866</v>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A525" s="7">
+        <v>42867</v>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A526" s="7">
+        <v>42868</v>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A527" s="7">
+        <v>42869</v>
+      </c>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A528" s="7">
+        <v>42870</v>
+      </c>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A529" s="7">
+        <v>42871</v>
+      </c>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A530" s="7">
+        <v>42872</v>
+      </c>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A531" s="7">
+        <v>42873</v>
+      </c>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A532" s="7">
+        <v>42874</v>
+      </c>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A533" s="7">
+        <v>42875</v>
+      </c>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A534" s="7">
+        <v>42876</v>
+      </c>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A535" s="7">
+        <v>42877</v>
+      </c>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A536" s="7">
+        <v>42878</v>
+      </c>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A537" s="7">
+        <v>42879</v>
+      </c>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A538" s="7">
+        <v>42880</v>
+      </c>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A539" s="7">
+        <v>42881</v>
+      </c>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A540" s="7">
+        <v>42882</v>
+      </c>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A541" s="7">
+        <v>42883</v>
+      </c>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A542" s="7">
+        <v>42884</v>
+      </c>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A543" s="7">
+        <v>42885</v>
+      </c>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A544" s="7">
+        <v>42886</v>
+      </c>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A545" s="7">
+        <v>42887</v>
+      </c>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A546" s="7">
+        <v>42888</v>
+      </c>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A547" s="7">
+        <v>42889</v>
+      </c>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A548" s="7">
+        <v>42890</v>
+      </c>
+    </row>
+    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A549" s="7">
+        <v>42891</v>
+      </c>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A550" s="7">
+        <v>42892</v>
+      </c>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A551" s="7">
+        <v>42893</v>
+      </c>
+    </row>
+    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A552" s="7">
+        <v>42894</v>
+      </c>
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A553" s="7">
+        <v>42895</v>
+      </c>
+    </row>
+    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A554" s="7">
+        <v>42896</v>
+      </c>
+    </row>
+    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A555" s="7">
+        <v>42897</v>
+      </c>
+    </row>
+    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A556" s="7">
+        <v>42898</v>
+      </c>
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A557" s="7">
+        <v>42899</v>
+      </c>
+    </row>
+    <row r="558" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A558" s="7">
+        <v>42900</v>
+      </c>
+    </row>
+    <row r="559" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A559" s="7">
+        <v>42901</v>
+      </c>
+    </row>
+    <row r="560" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A560" s="7">
+        <v>42902</v>
+      </c>
+    </row>
+    <row r="561" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A561" s="7">
+        <v>42903</v>
+      </c>
+    </row>
+    <row r="562" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A562" s="7">
+        <v>42904</v>
+      </c>
+    </row>
+    <row r="563" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A563" s="7">
+        <v>42905</v>
+      </c>
+    </row>
+    <row r="564" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A564" s="7">
+        <v>42906</v>
+      </c>
+    </row>
+    <row r="565" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A565" s="7">
+        <v>42907</v>
+      </c>
+    </row>
+    <row r="566" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A566" s="7">
+        <v>42908</v>
+      </c>
+    </row>
+    <row r="567" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A567" s="7">
+        <v>42909</v>
+      </c>
+    </row>
+    <row r="568" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A568" s="7">
+        <v>42910</v>
+      </c>
+    </row>
+    <row r="569" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A569" s="7">
+        <v>42911</v>
+      </c>
+    </row>
+    <row r="570" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A570" s="7">
+        <v>42912</v>
+      </c>
+    </row>
+    <row r="571" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A571" s="7">
+        <v>42913</v>
+      </c>
+    </row>
+    <row r="572" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A572" s="7">
+        <v>42914</v>
+      </c>
+    </row>
+    <row r="573" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A573" s="7">
+        <v>42915</v>
+      </c>
+    </row>
+    <row r="574" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A574" s="7">
+        <v>42916</v>
+      </c>
+    </row>
+    <row r="575" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A575" s="7">
+        <v>42917</v>
+      </c>
+    </row>
+    <row r="576" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A576" s="7">
+        <v>42918</v>
+      </c>
+    </row>
+    <row r="577" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A577" s="7">
+        <v>42919</v>
+      </c>
+    </row>
+    <row r="578" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A578" s="7">
+        <v>42920</v>
+      </c>
+    </row>
+    <row r="579" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A579" s="7">
+        <v>42921</v>
+      </c>
+    </row>
+    <row r="580" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A580" s="7">
+        <v>42922</v>
+      </c>
+    </row>
+    <row r="581" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A581" s="7">
+        <v>42923</v>
+      </c>
+    </row>
+    <row r="582" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A582" s="7">
+        <v>42924</v>
+      </c>
+    </row>
+    <row r="583" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A583" s="7">
+        <v>42925</v>
+      </c>
+    </row>
+    <row r="584" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A584" s="7">
+        <v>42926</v>
+      </c>
+    </row>
+    <row r="585" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A585" s="7">
+        <v>42927</v>
+      </c>
+    </row>
+    <row r="586" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A586" s="7">
+        <v>42928</v>
+      </c>
+    </row>
+    <row r="587" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A587" s="7">
+        <v>42929</v>
+      </c>
+    </row>
+    <row r="588" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A588" s="7">
+        <v>42930</v>
+      </c>
+    </row>
+    <row r="589" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A589" s="7">
+        <v>42931</v>
+      </c>
+    </row>
+    <row r="590" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A590" s="7">
+        <v>42932</v>
+      </c>
+    </row>
+    <row r="591" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A591" s="7">
+        <v>42933</v>
+      </c>
+    </row>
+    <row r="592" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A592" s="7">
+        <v>42934</v>
+      </c>
+    </row>
+    <row r="593" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A593" s="7">
+        <v>42935</v>
+      </c>
+    </row>
+    <row r="594" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A594" s="7">
+        <v>42936</v>
+      </c>
+    </row>
+    <row r="595" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A595" s="7">
+        <v>42937</v>
+      </c>
+    </row>
+    <row r="596" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A596" s="7">
+        <v>42938</v>
+      </c>
+    </row>
+    <row r="597" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A597" s="7">
+        <v>42939</v>
+      </c>
+    </row>
+    <row r="598" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A598" s="7">
+        <v>42940</v>
+      </c>
+    </row>
+    <row r="599" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A599" s="7">
+        <v>42941</v>
+      </c>
+    </row>
+    <row r="600" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A600" s="7">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="601" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A601" s="7">
+        <v>42943</v>
+      </c>
+    </row>
+    <row r="602" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A602" s="7">
+        <v>42944</v>
+      </c>
+    </row>
+    <row r="603" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A603" s="7">
+        <v>42945</v>
+      </c>
+    </row>
+    <row r="604" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A604" s="7">
+        <v>42946</v>
+      </c>
+    </row>
+    <row r="605" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A605" s="7">
+        <v>42947</v>
+      </c>
+    </row>
+    <row r="606" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A606" s="7">
+        <v>42948</v>
+      </c>
+    </row>
+    <row r="607" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A607" s="7">
+        <v>42949</v>
+      </c>
+    </row>
+    <row r="608" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A608" s="7">
+        <v>42950</v>
+      </c>
+    </row>
+    <row r="609" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A609" s="7">
+        <v>42951</v>
+      </c>
+    </row>
+    <row r="610" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A610" s="7">
+        <v>42952</v>
+      </c>
+    </row>
+    <row r="611" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A611" s="7">
+        <v>42953</v>
+      </c>
+    </row>
+    <row r="612" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A612" s="7">
+        <v>42954</v>
+      </c>
+    </row>
+    <row r="613" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A613" s="7">
+        <v>42955</v>
+      </c>
+    </row>
+    <row r="614" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A614" s="7">
+        <v>42956</v>
+      </c>
+    </row>
+    <row r="615" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A615" s="7">
+        <v>42957</v>
+      </c>
+    </row>
+    <row r="616" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A616" s="7">
+        <v>42958</v>
+      </c>
+    </row>
+    <row r="617" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A617" s="7">
+        <v>42959</v>
+      </c>
+    </row>
+    <row r="618" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A618" s="7">
+        <v>42960</v>
       </c>
     </row>
   </sheetData>
@@ -7501,7 +8831,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B320" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M337" sqref="M337"/>
+      <selection pane="bottomRight" activeCell="N344" sqref="N344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21654,67 +22984,262 @@
         <v>25</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>42705</v>
       </c>
-    </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B337">
+        <v>8.52</v>
+      </c>
+      <c r="C337">
+        <v>158</v>
+      </c>
+      <c r="D337">
+        <v>1.4</v>
+      </c>
+      <c r="E337" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="F337" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="G337">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="H337">
+        <v>138</v>
+      </c>
+      <c r="I337" t="s">
+        <v>0</v>
+      </c>
+      <c r="J337">
+        <v>1.58</v>
+      </c>
+      <c r="K337">
+        <v>5.26</v>
+      </c>
+      <c r="L337" s="20">
+        <v>47</v>
+      </c>
+      <c r="M337" s="20">
+        <v>23.91</v>
+      </c>
+      <c r="N337" s="20">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="338" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>42706</v>
       </c>
-    </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B338">
+        <v>8.48</v>
+      </c>
+      <c r="C338">
+        <v>148</v>
+      </c>
+      <c r="D338">
+        <v>1.35</v>
+      </c>
+      <c r="E338" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="F338" s="2">
+        <v>2.66</v>
+      </c>
+      <c r="G338">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="H338">
+        <v>117</v>
+      </c>
+      <c r="I338" t="s">
+        <v>0</v>
+      </c>
+      <c r="J338">
+        <v>1.51</v>
+      </c>
+      <c r="K338">
+        <v>5.16</v>
+      </c>
+      <c r="L338" s="20">
+        <v>39</v>
+      </c>
+      <c r="M338" s="20">
+        <v>23.86</v>
+      </c>
+      <c r="N338" s="20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="339" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>42707</v>
       </c>
-    </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B339">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="C339">
+        <v>139</v>
+      </c>
+      <c r="D339">
+        <v>1.3</v>
+      </c>
+      <c r="E339" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="F339" s="2">
+        <v>2.27</v>
+      </c>
+      <c r="G339">
+        <v>4.71</v>
+      </c>
+      <c r="H339">
+        <v>103</v>
+      </c>
+      <c r="I339" t="s">
+        <v>0</v>
+      </c>
+      <c r="J339">
+        <v>1.46</v>
+      </c>
+      <c r="K339">
+        <v>5.09</v>
+      </c>
+      <c r="L339" s="20">
+        <v>35</v>
+      </c>
+      <c r="M339" s="20">
+        <v>23.82</v>
+      </c>
+      <c r="N339" s="20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="340" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <v>42708</v>
       </c>
-    </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B340">
+        <v>8.44</v>
+      </c>
+      <c r="C340">
+        <v>137</v>
+      </c>
+      <c r="D340">
+        <v>1.26</v>
+      </c>
+      <c r="E340" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="F340" s="2">
+        <v>1.99</v>
+      </c>
+      <c r="G340">
+        <v>4.66</v>
+      </c>
+      <c r="H340">
+        <v>92</v>
+      </c>
+      <c r="I340" t="s">
+        <v>0</v>
+      </c>
+      <c r="J340">
+        <v>1.42</v>
+      </c>
+      <c r="K340">
+        <v>5.04</v>
+      </c>
+      <c r="L340" s="20">
+        <v>32</v>
+      </c>
+      <c r="M340" s="20">
+        <v>23.8</v>
+      </c>
+      <c r="N340" s="20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="341" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <v>42709</v>
       </c>
-    </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B341">
+        <v>8.42</v>
+      </c>
+      <c r="C341">
+        <v>132</v>
+      </c>
+      <c r="D341">
+        <v>1.23</v>
+      </c>
+      <c r="E341" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="F341" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="G341">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="H341">
+        <v>81</v>
+      </c>
+      <c r="I341" t="s">
+        <v>0</v>
+      </c>
+      <c r="J341">
+        <v>1.4</v>
+      </c>
+      <c r="K341">
+        <v>5</v>
+      </c>
+      <c r="L341" s="20">
+        <v>30</v>
+      </c>
+      <c r="M341" s="20">
+        <v>23.78</v>
+      </c>
+      <c r="N341" s="20">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="342" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <v>42710</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <v>42711</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <v>42712</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <v>42713</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <v>42714</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>42715</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>42716</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>42717</v>
       </c>

</xml_diff>